<commit_message>
Modifying Online Learning Dataset and 2-2 Factorial Design
</commit_message>
<xml_diff>
--- a/Assignments/HW2/Online Learning and Engagement.xlsx
+++ b/Assignments/HW2/Online Learning and Engagement.xlsx
@@ -1,21 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KSU\Teaching\STAT 7220\STAT-7220-Applied-Experimental-Design\STAT-7220-Applied-Experimental-Design\Assignments\HW2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC7C9A3-F6AC-4145-AD55-02DB550C44F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>Engagement</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Early Afternoon</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Mid Afternoon</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Evening</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +122,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +174,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +208,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +243,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,350 +419,253 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Day</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Section</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Platform</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Engagement</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
       <c r="D2">
         <v>1374.88</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Early Afternoon</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3">
         <v>1345.51</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Mid Afternoon</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>1277.89</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Monday</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Evening</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+        <v>1277.8900000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5">
         <v>1370.4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
       </c>
       <c r="D6">
         <v>1357.65</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Early Afternoon</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>1288.86</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Mid Afternoon</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+        <v>1288.8599999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>1298.6</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Evening</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+        <v>1298.5999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
       </c>
       <c r="D9">
         <v>1388.68</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
       </c>
       <c r="D10">
         <v>1397.12</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Early Afternoon</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
       </c>
       <c r="D11">
         <v>1340.77</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Mid Afternoon</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
       </c>
       <c r="D12">
         <v>1327.79</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Wednesday</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Evening</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
       </c>
       <c r="D13">
         <v>1356.74</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
       </c>
       <c r="D14">
         <v>1381.42</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Early Afternoon</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
       </c>
       <c r="D15">
         <v>1349.91</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Mid Afternoon</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
       </c>
       <c r="D16">
         <v>1311.01</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Evening</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
       </c>
       <c r="D17">
         <v>1363.47</v>

</xml_diff>